<commit_message>
feat: tune trafo book export layout
</commit_message>
<xml_diff>
--- a/src/assets/Book Fotográfico Empreiteiras - Trafos Queimados e Avariados - 9555.xlsx
+++ b/src/assets/Book Fotográfico Empreiteiras - Trafos Queimados e Avariados - 9555.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ENGENHARIA 11\Sistema_Obras\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ED61A1DE-4D59-4FE0-A373-072FF23BC277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39644208-1ABB-435E-A834-D8D44A7F91A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,10 +16,21 @@
     <sheet name="BOOK FOTOGRÁFICO" sheetId="1" r:id="rId1"/>
     <sheet name="LISTA DE FOTOS" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1047,138 +1058,6 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>504824</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>323849</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>2495625</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Imagem 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A14BE0C-6644-432B-8ED0-5174D806069E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6105524" y="10648950"/>
-          <a:ext cx="3476625" cy="2448000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>2505150</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="17" name="Imagem 16">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9949F2CE-B8D9-4832-92F8-A3C8D6081181}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6229350" y="5191125"/>
-          <a:ext cx="3257550" cy="2448000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>2505150</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="26" name="Imagem 25">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51D500C1-246F-4BC5-B352-A4CF3C39C313}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1171575" y="7924800"/>
-          <a:ext cx="3676650" cy="2448000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2622,7 +2501,7 @@
   <dimension ref="A1:U31"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>